<commit_message>
Added a very simple GUI. Still needs to be improved to be fully useable
</commit_message>
<xml_diff>
--- a/places_to_call.xlsx
+++ b/places_to_call.xlsx
@@ -1497,7 +1497,11 @@
           <t>5475 Rue des Jockeys, Montréal, QC H4P 2M1, Canada</t>
         </is>
       </c>
-      <c r="N17" t="inlineStr"/>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>2025-03-21 18:51: Hello | 2025-03-21 18:51: HELLOOOO</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">

</xml_diff>